<commit_message>
Casi cierre de CS_04_09_CO y Recepción de CS_06_04_CO
Versión editada de 04_09 y originales de autor 06_04
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion09/EsqueletoGuion_CS_04_09_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion09/EsqueletoGuion_CS_04_09_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="67">
   <si>
     <t>FICHA</t>
   </si>
@@ -218,13 +218,22 @@
   </si>
   <si>
     <t>Mapa Conceptual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los territorios indígenas </t>
+  </si>
+  <si>
+    <t>Competencias: Titulación colectiva de los territorios afrocolombianos</t>
+  </si>
+  <si>
+    <t>Competencias: Competencias: Titulación colectiva de los territorios afrocolombianos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,13 +282,6 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -774,9 +776,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -1460,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1611,12 +1615,12 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.140625" customWidth="1"/>
+    <col min="1" max="1" width="97.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1880,7 +1884,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
@@ -2288,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,7 +2838,7 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>27</v>
       </c>
       <c r="I24" s="9" t="s">
@@ -2964,7 +2968,7 @@
       <c r="D31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="19" t="s">
         <v>52</v>
       </c>
       <c r="H31" s="2"/>
@@ -2985,7 +2989,7 @@
       <c r="E32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I32" s="9" t="s">
@@ -3094,7 +3098,7 @@
       <c r="D38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="19" t="s">
         <v>52</v>
       </c>
       <c r="H38" s="2"/>
@@ -3152,7 +3156,7 @@
       <c r="D41" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="19" t="s">
         <v>52</v>
       </c>
       <c r="H41" s="2"/>
@@ -3170,7 +3174,7 @@
       <c r="D42" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="19" t="s">
         <v>51</v>
       </c>
       <c r="H42" s="2"/>
@@ -3189,14 +3193,10 @@
         <v>37</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>49</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="9"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
@@ -3211,10 +3211,10 @@
         <v>37</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>49</v>
@@ -3233,10 +3233,14 @@
         <v>37</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
@@ -3366,7 +3370,7 @@
       <c r="C53" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H53" s="17" t="s">
         <v>41</v>
       </c>
       <c r="I53" s="8" t="s">
@@ -3446,7 +3450,7 @@
         <v>54</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>49</v>
@@ -3511,9 +3515,25 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+      <c r="I61" s="8"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="8"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+      <c r="I63" s="8"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+      <c r="I64" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>